<commit_message>
isStraight replaced by findStraight; returns now the card straight List
</commit_message>
<xml_diff>
--- a/DefinitionEtSuiviDeTaches-v05.xlsx
+++ b/DefinitionEtSuiviDeTaches-v05.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27031"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unice-my.sharepoint.com/personal/antoine-marie_michelozzi_etu_unice_fr/Documents/SI3/Projet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lassa\Desktop\Cours\SI 3\PS5\Poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED8D5199-CAC7-46C7-90FB-A73B36ABE7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC6AC78-6F0D-4108-8BC4-0FA01617D415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>Définition</t>
   </si>
@@ -1882,13 +1882,39 @@
   </si>
   <si>
     <t>help</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/////////////////////////////// </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Passage au Jeu de Poker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ///////////////////////////////</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1966,6 +1992,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1993,7 +2034,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2014,6 +2055,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -2026,7 +2095,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2053,29 +2122,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2087,24 +2165,14 @@
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="12">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2195,56 +2263,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2546,41 +2564,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J475015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="66" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="13" customWidth="1"/>
-    <col min="2" max="2" width="60.125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="15.75" style="13" customWidth="1"/>
-    <col min="4" max="4" width="31.625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="29.5" style="13" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="13.875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13" style="13" customWidth="1"/>
-    <col min="10" max="16384" width="11" style="13"/>
+    <col min="1" max="1" width="7.5" style="11" customWidth="1"/>
+    <col min="2" max="2" width="60.09765625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="15.69921875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="31.59765625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="29.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.8984375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="13" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" ht="16.5">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2590,10 +2608,10 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2607,7 +2625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="64.5">
+    <row r="3" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>ROW(A3)-2</f>
         <v>1</v>
@@ -2637,7 +2655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="65.25" customHeight="1">
+    <row r="4" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A6" si="0">ROW(A4)-2</f>
         <v>2</v>
@@ -2667,7 +2685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="64.5">
+    <row r="5" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2695,7 +2713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="64.5">
+    <row r="6" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2725,7 +2743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="49.5" customHeight="1">
+    <row r="7" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2752,7 +2770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="46.5" customHeight="1">
+    <row r="8" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2779,7 +2797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="50.25" customHeight="1">
+    <row r="9" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2808,7 +2826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="81">
+    <row r="10" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2821,7 +2839,7 @@
       <c r="D10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -2837,7 +2855,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="81">
+    <row r="11" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2866,7 +2884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="81">
+    <row r="12" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2893,7 +2911,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="50.25" customHeight="1">
+    <row r="13" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2920,7 +2938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="61.5" customHeight="1">
+    <row r="14" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2947,7 +2965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="76.5" customHeight="1">
+    <row r="15" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2974,7 +2992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="88.5" customHeight="1">
+    <row r="16" spans="1:10" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3001,7 +3019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="73.5" customHeight="1">
+    <row r="17" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3030,7 +3048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="46.5" customHeight="1">
+    <row r="18" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3057,7 +3075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="101.25" customHeight="1">
+    <row r="19" spans="1:9" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3084,7 +3102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="87" customHeight="1">
+    <row r="20" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="37.5" customHeight="1">
+    <row r="21" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3136,7 +3154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="87" customHeight="1">
+    <row r="22" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3165,275 +3183,251 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="94.5" customHeight="1">
+    <row r="23" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="16"/>
+      <c r="F23" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="17">
         <v>45236</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="17">
         <v>45236</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="94.5" customHeight="1">
-      <c r="A24" s="13">
+    <row r="24" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
         <v>23</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="17"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A25" s="13">
+      <c r="B24" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A26" s="13">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A27" s="13">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A28" s="13">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="13">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="13">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A31" s="13">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A32" s="13">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A33" s="13">
+    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A34" s="13">
+    <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A35" s="13">
+    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A36" s="13">
+    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A37" s="13">
+    <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A38" s="13">
+    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A39" s="13">
+    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A40" s="13">
+    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="11">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A41" s="13">
+    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="11">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A42" s="13">
+    <row r="42" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A43" s="13">
+    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="11">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A44" s="13">
+    <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="11">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A45" s="13">
+    <row r="45" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="11">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A46" s="13">
+    <row r="46" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="11">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A47" s="13">
+    <row r="47" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="11">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A48" s="13">
+    <row r="48" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="11">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A49" s="13">
+    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="11">
         <v>48</v>
       </c>
     </row>
-    <row r="765" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B765" s="13" t="s">
+    <row r="765" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B765" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="475015" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B475015" s="13" t="s">
+    <row r="475015" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B475015" s="11" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B24:I24"/>
   </mergeCells>
-  <conditionalFormatting sqref="A4:A6 A3:F3 F2 A2:D2 F4:F7 E5:E7 D4:D11 H10:H14 A7:B14 I3:I24 B15:B21 G12:G24 A15:A24 D13:E24">
-    <cfRule type="cellIs" dxfId="17" priority="28" operator="equal">
+  <conditionalFormatting sqref="A2:D2 F2 A3:F3 I3:I23 A4:A6 F4:F7 E5:E7 A7:B14 H10:H14 G12:G23 D13:E23 B15:B21 A15:A24">
+    <cfRule type="cellIs" dxfId="11" priority="28" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:C4 A1:G1 B5:B6 E8:F8 E12:F12 F14:F15 F17 F19 F21 A25:G1048576 B22:C24 F23:F24 E4:F4 F9 F10:G11">
-    <cfRule type="cellIs" dxfId="16" priority="40" operator="equal">
+  <conditionalFormatting sqref="D4:D12">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F7 I3:I24">
-    <cfRule type="containsText" dxfId="15" priority="34" operator="containsText" text="PF">
+  <conditionalFormatting sqref="E9:E11">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:F4 F14:F15 F17 F19 F21 F23 A1:G1 B4:C4 B5:B6 E8:F8 F9 F10:G11 E12:F12 B22:C23 A25:G1048576 B24">
+    <cfRule type="cellIs" dxfId="8" priority="40" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 F16 F18 F20 F22">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:F15 F17 F19 F21 F23">
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",F14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:H9">
+    <cfRule type="cellIs" dxfId="5" priority="18" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:I2 J7:J24 H15:H19">
+    <cfRule type="cellIs" dxfId="4" priority="33" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:H23">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J1 H21 H25:J1048576">
+    <cfRule type="cellIs" dxfId="1" priority="37" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I23 F4:F7">
+    <cfRule type="containsText" dxfId="0" priority="34" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:I2 G3:H6 J7:J24 H15:H19">
-    <cfRule type="cellIs" dxfId="14" priority="33" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:J1 H25:J1048576 H21">
-    <cfRule type="cellIs" dxfId="13" priority="37" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G9">
-    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="11" priority="22" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13 F16 F18 F20 F22">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F15 F17 F19 F21 F23:F24">
-    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",F14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23:H24">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>